<commit_message>
update: add paper review
</commit_message>
<xml_diff>
--- a/Anying Xiang/SEP-B/Sprint 3/Experiment/Preparation/experiment preparation.xlsx
+++ b/Anying Xiang/SEP-B/Sprint 3/Experiment/Preparation/experiment preparation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\G-PostGraduate\SEP-B\Git-Project\Anying Xiang\SEP-B\Sprint 3\Exploration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\G-PostGraduate\SEP-B\Git-Project\Anying Xiang\SEP-B\Sprint 3\Experiment\Preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3FB4B-841B-4088-85A4-053A4F3E6340}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D5460F-5329-44BA-9AE8-6EA1A88A1B4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>spark.serializer</t>
   </si>
   <si>
-    <t>spark.reducer.maxSizeInFlight</t>
-  </si>
-  <si>
     <t>spark.shuffle.file.buffer</t>
   </si>
   <si>
@@ -116,10 +113,6 @@
   </si>
   <si>
     <t>32k</t>
-  </si>
-  <si>
-    <t>If set to higher value, the burden on memory, cpu and disk might be increased (use more memory, and thus more cpu and disk, memory is the bottleneck).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>If set to false, the burden on memory will be reduced, while the burden on net will be increased.</t>
@@ -198,6 +191,14 @@
       </rPr>
       <t>●</t>
     </r>
+  </si>
+  <si>
+    <t>spark.reducer.maxSizeInFlight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If set to higher value, the burden on memory and cpu might be increased (use more memory, and thus more cpu and disk, memory is the bottleneck).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -320,16 +321,7 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -342,6 +334,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -632,7 +633,7 @@
   <dimension ref="B1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -649,325 +650,325 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="I14" s="8" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>